<commit_message>
Changes in the flow
</commit_message>
<xml_diff>
--- a/HRBR Aug.xlsx
+++ b/HRBR Aug.xlsx
@@ -1169,12 +1169,12 @@
   <dimension ref="A1:Y1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5714285714286" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="19.5714285714286" customWidth="1"/>
     <col min="2" max="16384" width="15.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>